<commit_message>
update pinout files including switch overide
</commit_message>
<xml_diff>
--- a/main/Connectors_specs.xlsx
+++ b/main/Connectors_specs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eszte\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eszte\Desktop\UnlimitedRobotics\GIT\university_project\main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BAF6CC6-E787-4D04-A8C3-B127F495CEF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C11E16-3FC9-4209-9E43-D69F09CAEBB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="7360" xr2:uid="{6D40A45F-EDD9-4338-A3C0-75732E0DC9CF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6D40A45F-EDD9-4338-A3C0-75732E0DC9CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
   <si>
     <t>Board component</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>Pin's number</t>
+  </si>
+  <si>
+    <t>4,5,6</t>
   </si>
 </sst>
 </file>
@@ -161,7 +164,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,6 +183,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="42">
     <border>
@@ -708,17 +729,81 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -731,155 +816,68 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -887,18 +885,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -911,17 +903,59 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1244,8 +1278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4377B7C-6FF6-459E-BE32-C1E3B78AF46B}">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12:H19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24:J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1259,681 +1293,689 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="27"/>
-      <c r="B1" s="27"/>
+      <c r="A1" s="8"/>
+      <c r="B1" s="8"/>
     </row>
     <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
     </row>
     <row r="3" spans="1:11" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="1" t="s">
+      <c r="A3" s="48"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="2" t="s">
+      <c r="D3" s="13"/>
+      <c r="E3" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="1" t="s">
+      <c r="F3" s="13"/>
+      <c r="G3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="1" t="s">
+      <c r="H3" s="13"/>
+      <c r="I3" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="10" t="s">
+      <c r="J3" s="13"/>
+      <c r="K3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" s="27"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="4" t="s">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="29">
+      <c r="D4" s="27"/>
+      <c r="E4" s="22">
         <v>1</v>
       </c>
-      <c r="F4" s="24"/>
-      <c r="G4" s="52" t="s">
+      <c r="F4" s="23"/>
+      <c r="G4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="53"/>
-      <c r="I4" s="18">
+      <c r="H4" s="15"/>
+      <c r="I4" s="5">
         <v>1</v>
       </c>
-      <c r="J4" s="14">
+      <c r="J4" s="2">
         <v>5</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="72" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="6" t="s">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="30">
+      <c r="D5" s="29"/>
+      <c r="E5" s="24">
         <v>2</v>
       </c>
       <c r="F5" s="25"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="19">
+      <c r="G5" s="16"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="6">
         <v>2</v>
       </c>
-      <c r="J5" s="15">
+      <c r="J5" s="3">
         <v>9</v>
       </c>
-      <c r="K5" s="12"/>
+      <c r="K5" s="73"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="27"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="6" t="s">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="30">
+      <c r="D6" s="29"/>
+      <c r="E6" s="24">
         <v>3</v>
       </c>
       <c r="F6" s="25"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="19">
+      <c r="G6" s="16"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="6">
         <v>3</v>
       </c>
-      <c r="J6" s="15">
+      <c r="J6" s="3">
         <v>4</v>
       </c>
-      <c r="K6" s="12"/>
+      <c r="K6" s="73"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="6" t="s">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="30">
+      <c r="D7" s="29"/>
+      <c r="E7" s="24">
         <v>4</v>
       </c>
       <c r="F7" s="25"/>
-      <c r="G7" s="54"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="19">
+      <c r="G7" s="16"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="6">
         <v>4</v>
       </c>
-      <c r="J7" s="15">
+      <c r="J7" s="3">
         <v>8</v>
       </c>
-      <c r="K7" s="12"/>
+      <c r="K7" s="73"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="27"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="6" t="s">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="30">
+      <c r="D8" s="29"/>
+      <c r="E8" s="24">
         <v>5</v>
       </c>
       <c r="F8" s="25"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="55"/>
-      <c r="I8" s="19">
+      <c r="G8" s="16"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="6">
         <v>5</v>
       </c>
-      <c r="J8" s="15">
+      <c r="J8" s="3">
         <v>7</v>
       </c>
-      <c r="K8" s="12"/>
+      <c r="K8" s="73"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="27"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="6" t="s">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="30">
+      <c r="D9" s="29"/>
+      <c r="E9" s="24">
         <v>6</v>
       </c>
       <c r="F9" s="25"/>
-      <c r="G9" s="54"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="19">
+      <c r="G9" s="16"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="6">
         <v>6</v>
       </c>
-      <c r="J9" s="15">
+      <c r="J9" s="3">
         <v>2</v>
       </c>
-      <c r="K9" s="12"/>
+      <c r="K9" s="73"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="6" t="s">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="30">
+      <c r="D10" s="29"/>
+      <c r="E10" s="24">
         <v>7</v>
       </c>
       <c r="F10" s="25"/>
-      <c r="G10" s="54"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="19">
+      <c r="G10" s="16"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="6">
         <v>7</v>
       </c>
-      <c r="J10" s="15">
+      <c r="J10" s="3">
         <v>6</v>
       </c>
-      <c r="K10" s="12"/>
+      <c r="K10" s="73"/>
     </row>
     <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="27"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="8" t="s">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="31">
+      <c r="D11" s="33"/>
+      <c r="E11" s="30">
         <v>8</v>
       </c>
-      <c r="F11" s="26"/>
-      <c r="G11" s="56"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="20">
+      <c r="F11" s="31"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="7">
         <v>8</v>
       </c>
-      <c r="J11" s="16">
+      <c r="J11" s="4">
         <v>1</v>
       </c>
-      <c r="K11" s="13"/>
+      <c r="K11" s="74"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="27"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="4" t="s">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="32">
+      <c r="D12" s="27"/>
+      <c r="E12" s="38">
         <v>1</v>
       </c>
-      <c r="F12" s="21"/>
-      <c r="G12" s="54" t="s">
+      <c r="F12" s="39"/>
+      <c r="G12" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="H12" s="55"/>
-      <c r="I12" s="18">
+      <c r="H12" s="17"/>
+      <c r="I12" s="5">
         <v>1</v>
       </c>
-      <c r="J12" s="14">
+      <c r="J12" s="2">
         <v>1</v>
       </c>
-      <c r="K12" s="11" t="s">
+      <c r="K12" s="69" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="6" t="s">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="33">
+      <c r="D13" s="29"/>
+      <c r="E13" s="34">
         <v>2</v>
       </c>
-      <c r="F13" s="22"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="55"/>
-      <c r="I13" s="19">
+      <c r="F13" s="35"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="6">
         <v>2</v>
       </c>
-      <c r="J13" s="15" t="s">
+      <c r="J13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K13" s="12"/>
+      <c r="K13" s="71"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="27"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="6" t="s">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="33">
+      <c r="D14" s="29"/>
+      <c r="E14" s="34">
         <v>3</v>
       </c>
-      <c r="F14" s="22"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="55"/>
-      <c r="I14" s="19">
+      <c r="F14" s="35"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="6">
         <v>3</v>
       </c>
-      <c r="J14" s="15">
+      <c r="J14" s="3">
         <v>3</v>
       </c>
-      <c r="K14" s="12"/>
+      <c r="K14" s="71"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" s="27"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="6" t="s">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="33">
+      <c r="D15" s="29"/>
+      <c r="E15" s="34">
         <v>4</v>
       </c>
-      <c r="F15" s="22"/>
-      <c r="G15" s="54"/>
-      <c r="H15" s="55"/>
-      <c r="I15" s="19">
+      <c r="F15" s="35"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="6">
         <v>4</v>
       </c>
-      <c r="J15" s="15">
+      <c r="J15" s="3">
         <v>5</v>
       </c>
-      <c r="K15" s="12"/>
+      <c r="K15" s="71"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A16" s="27"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="6" t="s">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="33">
+      <c r="D16" s="29"/>
+      <c r="E16" s="34">
         <v>5</v>
       </c>
-      <c r="F16" s="22"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="55"/>
-      <c r="I16" s="19">
+      <c r="F16" s="35"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="6">
         <v>5</v>
       </c>
-      <c r="J16" s="15">
+      <c r="J16" s="3">
         <v>4</v>
       </c>
-      <c r="K16" s="12"/>
+      <c r="K16" s="71"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" s="27"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="6" t="s">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="33">
+      <c r="D17" s="29"/>
+      <c r="E17" s="34">
         <v>6</v>
       </c>
-      <c r="F17" s="22"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="55"/>
-      <c r="I17" s="19">
+      <c r="F17" s="35"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="6">
         <v>6</v>
       </c>
-      <c r="J17" s="15">
+      <c r="J17" s="3">
         <v>6</v>
       </c>
-      <c r="K17" s="12"/>
+      <c r="K17" s="71"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="27"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="6" t="s">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="33">
+      <c r="D18" s="29"/>
+      <c r="E18" s="34">
         <v>7</v>
       </c>
-      <c r="F18" s="22"/>
-      <c r="G18" s="54"/>
-      <c r="H18" s="55"/>
-      <c r="I18" s="19">
+      <c r="F18" s="35"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="6">
         <v>7</v>
       </c>
-      <c r="J18" s="15">
+      <c r="J18" s="3">
         <v>7</v>
       </c>
-      <c r="K18" s="12"/>
+      <c r="K18" s="71"/>
     </row>
     <row r="19" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="8" t="s">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="34">
+      <c r="D19" s="33"/>
+      <c r="E19" s="36">
         <v>8</v>
       </c>
-      <c r="F19" s="23"/>
-      <c r="G19" s="54"/>
-      <c r="H19" s="55"/>
-      <c r="I19" s="20">
+      <c r="F19" s="37"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="7">
         <v>8</v>
       </c>
-      <c r="J19" s="16" t="s">
+      <c r="J19" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="K19" s="13"/>
+      <c r="K19" s="70"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" s="27"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="58" t="s">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="59"/>
-      <c r="E20" s="60">
+      <c r="D20" s="45"/>
+      <c r="E20" s="51">
         <v>1</v>
       </c>
-      <c r="F20" s="61"/>
-      <c r="G20" s="52" t="s">
+      <c r="F20" s="52"/>
+      <c r="G20" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="H20" s="53"/>
-      <c r="I20" s="18">
+      <c r="H20" s="15"/>
+      <c r="I20" s="5">
         <v>1</v>
       </c>
-      <c r="J20" s="72">
+      <c r="J20" s="10">
         <v>5</v>
       </c>
-      <c r="K20" s="70" t="s">
+      <c r="K20" s="20" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="27"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="17" t="s">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="36"/>
-      <c r="E21" s="37">
+      <c r="D21" s="47"/>
+      <c r="E21" s="40">
         <v>2</v>
       </c>
-      <c r="F21" s="38"/>
-      <c r="G21" s="56"/>
-      <c r="H21" s="57"/>
-      <c r="I21" s="35">
+      <c r="F21" s="41"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="9">
         <v>2</v>
       </c>
-      <c r="J21" s="73">
+      <c r="J21" s="11">
         <v>6</v>
       </c>
-      <c r="K21" s="71"/>
+      <c r="K21" s="21"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A22" s="27"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="4" t="s">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="47">
+      <c r="D22" s="27"/>
+      <c r="E22" s="42">
         <v>1</v>
       </c>
-      <c r="F22" s="21"/>
-      <c r="G22" s="52" t="s">
+      <c r="F22" s="39"/>
+      <c r="G22" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="H22" s="53"/>
-      <c r="I22" s="18">
+      <c r="H22" s="15"/>
+      <c r="I22" s="5">
         <v>1</v>
       </c>
-      <c r="J22" s="14" t="s">
+      <c r="J22" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K22" s="11" t="s">
+      <c r="K22" s="69" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="27"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="8" t="s">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="48">
+      <c r="D23" s="33"/>
+      <c r="E23" s="43">
         <v>2</v>
       </c>
-      <c r="F23" s="38"/>
-      <c r="G23" s="56"/>
-      <c r="H23" s="57"/>
-      <c r="I23" s="20">
+      <c r="F23" s="41"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="7">
         <v>2</v>
       </c>
-      <c r="J23" s="16" t="s">
+      <c r="J23" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K23" s="13"/>
+      <c r="K23" s="70"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A24" s="27"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="50" t="s">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="62"/>
-      <c r="E24" s="47">
+      <c r="D24" s="61"/>
+      <c r="E24" s="42">
         <v>1</v>
       </c>
-      <c r="F24" s="21"/>
-      <c r="G24" s="63" t="s">
+      <c r="F24" s="39"/>
+      <c r="G24" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="H24" s="64"/>
-      <c r="I24" s="18">
+      <c r="H24" s="54"/>
+      <c r="I24" s="5">
         <v>1</v>
       </c>
-      <c r="J24" s="14"/>
-      <c r="K24" s="40" t="s">
+      <c r="J24" s="2"/>
+      <c r="K24" s="66" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C25" s="43" t="s">
+      <c r="C25" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="45"/>
-      <c r="E25" s="65">
+      <c r="D25" s="63"/>
+      <c r="E25" s="50">
         <v>2</v>
       </c>
-      <c r="F25" s="22"/>
-      <c r="G25" s="66"/>
-      <c r="H25" s="67"/>
-      <c r="I25" s="19">
+      <c r="F25" s="35"/>
+      <c r="G25" s="55"/>
+      <c r="H25" s="56"/>
+      <c r="I25" s="6">
         <v>2</v>
       </c>
-      <c r="J25" s="15"/>
-      <c r="K25" s="41"/>
+      <c r="J25" s="3">
+        <v>1</v>
+      </c>
+      <c r="K25" s="67"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C26" s="43" t="s">
+      <c r="C26" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="45"/>
-      <c r="E26" s="65">
+      <c r="D26" s="63"/>
+      <c r="E26" s="50">
         <v>3</v>
       </c>
-      <c r="F26" s="22"/>
-      <c r="G26" s="66"/>
-      <c r="H26" s="67"/>
-      <c r="I26" s="19">
+      <c r="F26" s="35"/>
+      <c r="G26" s="55"/>
+      <c r="H26" s="56"/>
+      <c r="I26" s="6">
         <v>3</v>
       </c>
-      <c r="J26" s="15"/>
-      <c r="K26" s="41"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="67"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C27" s="43" t="s">
+      <c r="C27" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="45"/>
-      <c r="E27" s="65">
+      <c r="D27" s="63"/>
+      <c r="E27" s="50">
         <v>4</v>
       </c>
-      <c r="F27" s="22"/>
-      <c r="G27" s="66"/>
-      <c r="H27" s="67"/>
-      <c r="I27" s="19">
+      <c r="F27" s="35"/>
+      <c r="G27" s="55"/>
+      <c r="H27" s="56"/>
+      <c r="I27" s="6">
         <v>4</v>
       </c>
-      <c r="J27" s="15"/>
-      <c r="K27" s="41"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="67"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C28" s="43" t="s">
+      <c r="C28" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="D28" s="45"/>
-      <c r="E28" s="65">
+      <c r="D28" s="63"/>
+      <c r="E28" s="50">
         <v>5</v>
       </c>
-      <c r="F28" s="22"/>
-      <c r="G28" s="66"/>
-      <c r="H28" s="67"/>
-      <c r="I28" s="19">
+      <c r="F28" s="35"/>
+      <c r="G28" s="55"/>
+      <c r="H28" s="56"/>
+      <c r="I28" s="6">
         <v>5</v>
       </c>
-      <c r="J28" s="15"/>
-      <c r="K28" s="41"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="67"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C29" s="43" t="s">
+      <c r="C29" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="D29" s="45"/>
-      <c r="E29" s="65">
+      <c r="D29" s="63"/>
+      <c r="E29" s="50">
         <v>6</v>
       </c>
-      <c r="F29" s="22"/>
-      <c r="G29" s="66"/>
-      <c r="H29" s="67"/>
-      <c r="I29" s="19">
+      <c r="F29" s="35"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="56"/>
+      <c r="I29" s="6">
         <v>6</v>
       </c>
-      <c r="J29" s="15"/>
-      <c r="K29" s="41"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="67"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C30" s="43" t="s">
+      <c r="C30" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="45"/>
-      <c r="E30" s="65">
+      <c r="D30" s="63"/>
+      <c r="E30" s="50">
         <v>7</v>
       </c>
-      <c r="F30" s="22"/>
-      <c r="G30" s="66"/>
-      <c r="H30" s="67"/>
-      <c r="I30" s="19">
+      <c r="F30" s="35"/>
+      <c r="G30" s="55"/>
+      <c r="H30" s="56"/>
+      <c r="I30" s="6">
         <v>7</v>
       </c>
-      <c r="J30" s="15"/>
-      <c r="K30" s="41"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="67"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C31" s="43" t="s">
+      <c r="C31" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="45"/>
-      <c r="E31" s="65">
+      <c r="D31" s="63"/>
+      <c r="E31" s="50">
         <v>8</v>
       </c>
-      <c r="F31" s="22"/>
-      <c r="G31" s="66"/>
-      <c r="H31" s="67"/>
-      <c r="I31" s="19">
+      <c r="F31" s="35"/>
+      <c r="G31" s="55"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="6">
         <v>8</v>
       </c>
-      <c r="J31" s="15"/>
-      <c r="K31" s="41"/>
+      <c r="J31" s="3">
+        <v>2</v>
+      </c>
+      <c r="K31" s="67"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C32" s="43" t="s">
+      <c r="C32" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="D32" s="45"/>
-      <c r="E32" s="65">
+      <c r="D32" s="63"/>
+      <c r="E32" s="50">
         <v>9</v>
       </c>
-      <c r="F32" s="22"/>
-      <c r="G32" s="66"/>
-      <c r="H32" s="67"/>
-      <c r="I32" s="19">
+      <c r="F32" s="35"/>
+      <c r="G32" s="55"/>
+      <c r="H32" s="56"/>
+      <c r="I32" s="6">
         <v>9</v>
       </c>
-      <c r="J32" s="39"/>
-      <c r="K32" s="41"/>
+      <c r="J32" s="75"/>
+      <c r="K32" s="67"/>
     </row>
     <row r="33" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C33" s="43" t="s">
+      <c r="C33" s="62" t="s">
         <v>31</v>
       </c>
-      <c r="D33" s="45"/>
-      <c r="E33" s="65">
+      <c r="D33" s="63"/>
+      <c r="E33" s="50">
         <v>10</v>
       </c>
-      <c r="F33" s="22"/>
-      <c r="G33" s="66"/>
-      <c r="H33" s="67"/>
-      <c r="I33" s="19">
+      <c r="F33" s="35"/>
+      <c r="G33" s="55"/>
+      <c r="H33" s="56"/>
+      <c r="I33" s="6">
         <v>10</v>
       </c>
-      <c r="J33" s="39"/>
-      <c r="K33" s="41"/>
+      <c r="J33" s="75">
+        <v>3</v>
+      </c>
+      <c r="K33" s="67"/>
     </row>
     <row r="34" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C34" s="43" t="s">
+      <c r="C34" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="45"/>
-      <c r="E34" s="65">
+      <c r="D34" s="63"/>
+      <c r="E34" s="50">
         <v>11</v>
       </c>
-      <c r="F34" s="22"/>
-      <c r="G34" s="66"/>
-      <c r="H34" s="67"/>
-      <c r="I34" s="19">
+      <c r="F34" s="35"/>
+      <c r="G34" s="55"/>
+      <c r="H34" s="56"/>
+      <c r="I34" s="6">
         <v>11</v>
       </c>
-      <c r="J34" s="39"/>
-      <c r="K34" s="41"/>
+      <c r="J34" s="75"/>
+      <c r="K34" s="67"/>
     </row>
     <row r="35" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C35" s="44" t="s">
+      <c r="C35" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="D35" s="46"/>
-      <c r="E35" s="49">
+      <c r="D35" s="65"/>
+      <c r="E35" s="59">
         <v>12</v>
       </c>
-      <c r="F35" s="23"/>
-      <c r="G35" s="68"/>
-      <c r="H35" s="69"/>
-      <c r="I35" s="20">
+      <c r="F35" s="37"/>
+      <c r="G35" s="57"/>
+      <c r="H35" s="58"/>
+      <c r="I35" s="7">
         <v>12</v>
       </c>
-      <c r="J35" s="51"/>
-      <c r="K35" s="42"/>
+      <c r="J35" s="76" t="s">
+        <v>35</v>
+      </c>
+      <c r="K35" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="79">

</xml_diff>